<commit_message>
Finished visualizing missing data
</commit_message>
<xml_diff>
--- a/dataSet/cleanData/missingData.xlsx
+++ b/dataSet/cleanData/missingData.xlsx
@@ -457,17 +457,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Broj oporavljenih osoba</t>
+          <t>Oporavljeni</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Broj testiranih dnevno</t>
+          <t>Testirani</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Broj smrtnih slučajeva</t>
+          <t>Smrtni sl.</t>
         </is>
       </c>
     </row>

</xml_diff>